<commit_message>
1. Submit test cases 2. Update milestone document with status
Signed-off-by: mishradileep <mishradileep@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/mishradileep_drupal_module_file_berth_milestones1.0.xlsx
+++ b/docs/mishradileep_drupal_module_file_berth_milestones1.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Task</t>
   </si>
@@ -110,13 +110,16 @@
   </si>
   <si>
     <t>Module Submit to Community</t>
+  </si>
+  <si>
+    <t>Not Required</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,16 +127,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -141,13 +170,159 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,183 +617,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D17"/>
+  <dimension ref="B1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="1" spans="2:5" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:5" ht="15.75" thickTop="1">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="3" spans="2:5">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="6">
         <v>41197</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="4" spans="2:5">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="6">
         <v>41198</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="E4" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="6">
         <v>41199</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="E5" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="6">
         <v>41200</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="6">
         <v>41202</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="6">
         <v>41205</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="6">
         <v>41206</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="6">
         <v>41207</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="6">
         <v>41208</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="6">
         <v>41210</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="6">
         <v>41212</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="6">
         <v>41213</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B17" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>